<commit_message>
updated BOM and changed on capacitor
</commit_message>
<xml_diff>
--- a/Projects/Main/Main.xlsx
+++ b/Projects/Main/Main.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuille1!$A$1:$E$23</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -124,10 +127,10 @@
     <t xml:space="preserve">DIP Socket 2x20,15.24 mm</t>
   </si>
   <si>
-    <t xml:space="preserve">K331K15X7RH53L2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - Leaded 330pF 100volts 10% X7R 2.5mm LS</t>
+    <t xml:space="preserve">FG18C0G1H331JNT00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - Leaded RAD 50V 330pF C0G 5% LS:2.5mm</t>
   </si>
   <si>
     <t xml:space="preserve">MF1/4CCT52R2200F</t>
@@ -274,23 +277,27 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="77.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="77.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.1"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
@@ -367,7 +374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>11</v>
       </c>
@@ -385,7 +392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>13</v>
       </c>
@@ -403,7 +410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>15</v>
       </c>
@@ -421,7 +428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>17</v>
       </c>
@@ -439,7 +446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>19</v>
       </c>
@@ -457,7 +464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>21</v>
       </c>
@@ -475,7 +482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>23</v>
       </c>
@@ -493,7 +500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>25</v>
       </c>
@@ -511,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>27</v>
       </c>
@@ -529,7 +536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>29</v>
       </c>
@@ -547,7 +554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
         <v>2222</v>
       </c>
@@ -565,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
@@ -601,7 +608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>36</v>
       </c>
@@ -673,7 +680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>44</v>
       </c>
@@ -710,6 +717,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E23">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="1"/>
+        <filter val="4"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -717,5 +732,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>